<commit_message>
new, much more efficient model with pallets as inputs
</commit_message>
<xml_diff>
--- a/problems/demands/0226.xlsx
+++ b/problems/demands/0226.xlsx
@@ -908,7 +908,7 @@
         <v>31</v>
       </c>
       <c r="B29" s="4">
-        <v>704</v>
+        <v>0</v>
       </c>
       <c r="C29" s="4">
         <v>407</v>
@@ -922,7 +922,7 @@
         <v>32</v>
       </c>
       <c r="B30" s="4">
-        <v>511</v>
+        <v>0</v>
       </c>
       <c r="C30" s="4">
         <v>234</v>

</xml_diff>